<commit_message>
OS combination for execution
</commit_message>
<xml_diff>
--- a/Crate/ParallelRun/Main.rvl.xlsx
+++ b/Crate/ParallelRun/Main.rvl.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="82">
   <si>
     <t>Flow</t>
   </si>
@@ -223,6 +223,42 @@
   </si>
   <si>
     <t>%WORKDIR%\TC_Signup\TC_Signup.sstest</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>robin133</t>
+  </si>
+  <si>
+    <t>robin133@crate.com</t>
+  </si>
+  <si>
+    <t>robin141</t>
+  </si>
+  <si>
+    <t>robin141@crate.com</t>
+  </si>
+  <si>
+    <t>iOS14.3</t>
+  </si>
+  <si>
+    <t>robin143</t>
+  </si>
+  <si>
+    <t>robin143@crate.com</t>
+  </si>
+  <si>
+    <t>iOS14.0</t>
+  </si>
+  <si>
+    <t>robin140</t>
+  </si>
+  <si>
+    <t>robin140@crate.com</t>
+  </si>
+  <si>
+    <t>@os='ios' and @version='14.0' and @category='PHONE'</t>
   </si>
 </sst>
 </file>
@@ -243,7 +279,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="169">
+  <borders count="176">
     <border>
       <left/>
       <right/>
@@ -419,11 +455,18 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="169">
+  <cellXfs count="176">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0"/>
@@ -593,6 +636,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="166" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="167" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="168" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="169" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="170" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="171" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="172" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="173" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="174" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="175" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -699,45 +749,45 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="168"/>
+      <c r="A5" s="162" t="s">
+        <v>7</v>
+      </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C5" t="s">
-        <v>65</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="E5" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="F5" t="s">
         <v>39</v>
       </c>
+      <c r="G5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" s="162" t="s">
-        <v>7</v>
-      </c>
+      <c r="A6" s="172"/>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>81</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>79</v>
       </c>
       <c r="E6" t="s">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="F6" t="s">
         <v>39</v>
       </c>
-      <c r="G6" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" s="163" t="s">
@@ -750,10 +800,10 @@
         <v>58</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
       <c r="E7" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="F7" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
Test Matrix as attachment in Spira
</commit_message>
<xml_diff>
--- a/Crate/ParallelRun/Main.rvl.xlsx
+++ b/Crate/ParallelRun/Main.rvl.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="109">
   <si>
     <t>Flow</t>
   </si>
@@ -292,6 +292,54 @@
   </si>
   <si>
     <t>LastResult</t>
+  </si>
+  <si>
+    <t>SeeTestLOcal</t>
+  </si>
+  <si>
+    <t>SLocal</t>
+  </si>
+  <si>
+    <t>BLocal</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>fileName</t>
+  </si>
+  <si>
+    <t>Data.xlsx</t>
+  </si>
+  <si>
+    <t>sheetName</t>
+  </si>
+  <si>
+    <t>Sheet1</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>ST_Rapise</t>
+  </si>
+  <si>
+    <t>BS_Rapise</t>
+  </si>
+  <si>
+    <t>ST_Spira</t>
+  </si>
+  <si>
+    <t>%ARTIFACTS%\TestMatrix.xlsx</t>
+  </si>
+  <si>
+    <t>SeeTest</t>
+  </si>
+  <si>
+    <t>BS_Spira</t>
+  </si>
+  <si>
+    <t>Browserstack</t>
   </si>
 </sst>
 </file>
@@ -312,7 +360,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="195">
+  <borders count="214">
     <border>
       <left/>
       <right/>
@@ -514,11 +562,30 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="195">
+  <cellXfs count="214">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0"/>
@@ -714,6 +781,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="192" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="193" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="194" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="195" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="196" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="197" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="198" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="199" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="200" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="201" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="202" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="203" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="204" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="205" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="206" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="207" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="208" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="209" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="210" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="211" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="212" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="213" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -723,7 +809,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:H44"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.5546875" customWidth="true"/>
@@ -819,7 +905,7 @@
         <v>9</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>82</v>
+        <v>102</v>
       </c>
       <c r="D7" s="20" t="s">
         <v>7</v>
@@ -956,7 +1042,7 @@
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="D14" t="s">
         <v>7</v>
@@ -1062,191 +1148,319 @@
       <c r="A19" s="184"/>
     </row>
     <row r="20">
-      <c r="A20" s="25"/>
-      <c r="B20" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="D20" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="E20" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="F20" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="G20" s="31" t="s">
-        <v>90</v>
-      </c>
-      <c r="H20" s="32"/>
+      <c r="A20" s="195" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20" t="s">
+        <v>104</v>
+      </c>
+      <c r="D20" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" t="s">
+        <v>97</v>
+      </c>
+      <c r="F20" t="s">
+        <v>46</v>
+      </c>
+      <c r="G20" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="21">
-      <c r="A21" s="166"/>
+      <c r="A21" s="205"/>
       <c r="B21" t="s">
         <v>47</v>
       </c>
       <c r="E21" t="s">
+        <v>99</v>
+      </c>
+      <c r="F21" t="s">
+        <v>46</v>
+      </c>
+      <c r="G21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="203" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="204"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="196" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" t="s">
+        <v>96</v>
+      </c>
+      <c r="C24" t="s">
+        <v>107</v>
+      </c>
+      <c r="D24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" t="s">
+        <v>97</v>
+      </c>
+      <c r="F24" t="s">
+        <v>46</v>
+      </c>
+      <c r="G24" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="211"/>
+      <c r="B25" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" t="s">
+        <v>99</v>
+      </c>
+      <c r="F25" t="s">
+        <v>46</v>
+      </c>
+      <c r="G25" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="209" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="210"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="25"/>
+      <c r="B28" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="E28" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="F28" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="G28" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="H28" s="32"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="166"/>
+      <c r="B29" t="s">
+        <v>47</v>
+      </c>
+      <c r="E29" t="s">
         <v>48</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F29" t="s">
         <v>49</v>
       </c>
-      <c r="G21" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="33"/>
-      <c r="B22" s="34"/>
-      <c r="C22" s="35"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="38"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="40"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="49"/>
-      <c r="B23" s="50"/>
-      <c r="C23" s="51"/>
-      <c r="D23" s="52"/>
-      <c r="E23" s="53"/>
-      <c r="F23" s="54"/>
-      <c r="G23" s="55"/>
-      <c r="H23" s="56"/>
-    </row>
-    <row r="24">
-      <c r="A24" s="57"/>
-      <c r="B24" s="58"/>
-      <c r="C24" s="59"/>
-      <c r="D24" s="60"/>
-      <c r="E24" s="61"/>
-      <c r="F24" s="62"/>
-      <c r="G24" s="63"/>
-      <c r="H24" s="64"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="65"/>
-      <c r="B25" s="66"/>
-      <c r="C25" s="67"/>
-      <c r="D25" s="68"/>
-      <c r="E25" s="69"/>
-      <c r="F25" s="70"/>
-      <c r="G25" s="71"/>
-      <c r="H25" s="72"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="73"/>
-      <c r="B26" s="74"/>
-      <c r="C26" s="75"/>
-      <c r="D26" s="76"/>
-      <c r="E26" s="77"/>
-      <c r="F26" s="78"/>
-      <c r="G26" s="79"/>
-      <c r="H26" s="80"/>
-    </row>
-    <row r="27">
-      <c r="A27" s="81"/>
-      <c r="B27" s="82"/>
-      <c r="C27" s="83"/>
-      <c r="D27" s="84"/>
-      <c r="E27" s="85"/>
-      <c r="F27" s="86"/>
-      <c r="G27" s="87"/>
-      <c r="H27" s="88"/>
-    </row>
-    <row r="28">
-      <c r="A28" s="89"/>
-      <c r="B28" s="90"/>
-      <c r="C28" s="91"/>
-      <c r="D28" s="92"/>
-      <c r="E28" s="93"/>
-      <c r="F28" s="94"/>
-      <c r="G28" s="95"/>
-      <c r="H28" s="96"/>
-    </row>
-    <row r="29">
-      <c r="A29" s="97"/>
-      <c r="B29" s="98"/>
-      <c r="C29" s="99"/>
-      <c r="D29" s="100"/>
-      <c r="E29" s="101"/>
-      <c r="F29" s="102"/>
-      <c r="G29" s="103"/>
-      <c r="H29" s="104"/>
+      <c r="G29" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="30">
-      <c r="A30" s="105"/>
-      <c r="B30" s="106"/>
-      <c r="C30" s="107"/>
-      <c r="D30" s="108"/>
-      <c r="E30" s="109"/>
-      <c r="F30" s="110"/>
-      <c r="G30" s="111"/>
-      <c r="H30" s="112"/>
+      <c r="A30" s="33"/>
+      <c r="B30" s="34"/>
+      <c r="C30" s="35"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="40"/>
     </row>
     <row r="31">
-      <c r="A31" s="113"/>
-      <c r="B31" s="114"/>
-      <c r="C31" s="115"/>
-      <c r="D31" s="116"/>
-      <c r="E31" s="117"/>
-      <c r="F31" s="118"/>
-      <c r="G31" s="119"/>
-      <c r="H31" s="120"/>
+      <c r="A31" s="49"/>
+      <c r="B31" s="50"/>
+      <c r="C31" s="51"/>
+      <c r="D31" s="52"/>
+      <c r="E31" s="53"/>
+      <c r="F31" s="54"/>
+      <c r="G31" s="55"/>
+      <c r="H31" s="56"/>
     </row>
     <row r="32">
-      <c r="A32" s="121"/>
-      <c r="B32" s="122"/>
-      <c r="C32" s="123"/>
-      <c r="D32" s="124"/>
-      <c r="E32" s="125"/>
-      <c r="F32" s="126"/>
-      <c r="G32" s="127"/>
-      <c r="H32" s="128"/>
+      <c r="A32" s="57"/>
+      <c r="B32" s="58"/>
+      <c r="C32" s="59"/>
+      <c r="D32" s="60"/>
+      <c r="E32" s="61"/>
+      <c r="F32" s="62"/>
+      <c r="G32" s="63"/>
+      <c r="H32" s="64"/>
     </row>
     <row r="33">
-      <c r="A33" s="129"/>
-      <c r="B33" s="130"/>
-      <c r="C33" s="131"/>
-      <c r="D33" s="132"/>
-      <c r="E33" s="133"/>
-      <c r="F33" s="134"/>
-      <c r="G33" s="135"/>
-      <c r="H33" s="136"/>
+      <c r="A33" s="65"/>
+      <c r="B33" s="66"/>
+      <c r="C33" s="67"/>
+      <c r="D33" s="68"/>
+      <c r="E33" s="69"/>
+      <c r="F33" s="70"/>
+      <c r="G33" s="71"/>
+      <c r="H33" s="72"/>
     </row>
     <row r="34">
-      <c r="A34" s="137"/>
-      <c r="B34" s="138"/>
-      <c r="C34" s="139"/>
-      <c r="D34" s="140"/>
-      <c r="E34" s="141"/>
-      <c r="F34" s="142"/>
-      <c r="G34" s="143"/>
-      <c r="H34" s="144"/>
+      <c r="A34" s="73"/>
+      <c r="B34" s="74"/>
+      <c r="C34" s="75"/>
+      <c r="D34" s="76"/>
+      <c r="E34" s="77"/>
+      <c r="F34" s="78"/>
+      <c r="G34" s="79"/>
+      <c r="H34" s="80"/>
     </row>
     <row r="35">
-      <c r="A35" s="145"/>
-      <c r="B35" s="146"/>
-      <c r="C35" s="147"/>
-      <c r="D35" s="148"/>
-      <c r="E35" s="149"/>
-      <c r="F35" s="150"/>
-      <c r="G35" s="151"/>
-      <c r="H35" s="152"/>
+      <c r="A35" s="81"/>
+      <c r="B35" s="82"/>
+      <c r="C35" s="83"/>
+      <c r="D35" s="84"/>
+      <c r="E35" s="85"/>
+      <c r="F35" s="86"/>
+      <c r="G35" s="87"/>
+      <c r="H35" s="88"/>
     </row>
     <row r="36">
-      <c r="A36" s="153"/>
-      <c r="B36" s="154"/>
-      <c r="C36" s="155"/>
-      <c r="D36" s="156"/>
-      <c r="E36" s="157"/>
-      <c r="F36" s="158"/>
-      <c r="G36" s="159"/>
-      <c r="H36" s="160"/>
+      <c r="A36" s="89"/>
+      <c r="B36" s="90"/>
+      <c r="C36" s="91"/>
+      <c r="D36" s="92"/>
+      <c r="E36" s="93"/>
+      <c r="F36" s="94"/>
+      <c r="G36" s="95"/>
+      <c r="H36" s="96"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="97"/>
+      <c r="B37" s="98"/>
+      <c r="C37" s="99"/>
+      <c r="D37" s="100"/>
+      <c r="E37" s="101"/>
+      <c r="F37" s="102"/>
+      <c r="G37" s="103"/>
+      <c r="H37" s="104"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="105"/>
+      <c r="B38" s="106"/>
+      <c r="C38" s="107"/>
+      <c r="D38" s="108"/>
+      <c r="E38" s="109"/>
+      <c r="F38" s="110"/>
+      <c r="G38" s="111"/>
+      <c r="H38" s="112"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="113"/>
+      <c r="B39" s="114"/>
+      <c r="C39" s="115"/>
+      <c r="D39" s="116"/>
+      <c r="E39" s="117"/>
+      <c r="F39" s="118"/>
+      <c r="G39" s="119"/>
+      <c r="H39" s="120"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="121"/>
+      <c r="B40" s="122"/>
+      <c r="C40" s="123"/>
+      <c r="D40" s="124"/>
+      <c r="E40" s="125"/>
+      <c r="F40" s="126"/>
+      <c r="G40" s="127"/>
+      <c r="H40" s="128"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="129"/>
+      <c r="B41" s="130"/>
+      <c r="C41" s="131"/>
+      <c r="D41" s="132"/>
+      <c r="E41" s="133"/>
+      <c r="F41" s="134"/>
+      <c r="G41" s="135"/>
+      <c r="H41" s="136"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="137"/>
+      <c r="B42" s="138"/>
+      <c r="C42" s="139"/>
+      <c r="D42" s="140"/>
+      <c r="E42" s="141"/>
+      <c r="F42" s="142"/>
+      <c r="G42" s="143"/>
+      <c r="H42" s="144"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="145"/>
+      <c r="B43" s="146"/>
+      <c r="C43" s="147"/>
+      <c r="D43" s="148"/>
+      <c r="E43" s="149"/>
+      <c r="F43" s="150"/>
+      <c r="G43" s="151"/>
+      <c r="H43" s="152"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="153"/>
+      <c r="B44" s="154"/>
+      <c r="C44" s="155"/>
+      <c r="D44" s="156"/>
+      <c r="E44" s="157"/>
+      <c r="F44" s="158"/>
+      <c r="G44" s="159"/>
+      <c r="H44" s="160"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>